<commit_message>
Finalisation des logs + Grille aléatoire
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Scénarios_teste.xlsx
+++ b/Doccument_théorique/Scénarios_teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Schwartz\Documents\GitHub\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{86104F76-CC9C-478C-8A34-4025D057BFF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFC3626-ED67-4971-913B-353388C29635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-84" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,6 @@
     <t>Kenan</t>
   </si>
   <si>
-    <t>Arthur
-HP ENVY</t>
-  </si>
-  <si>
     <t>Léa</t>
   </si>
   <si>
@@ -70,9 +66,6 @@
     <t>1.2 Lisez les règle et appuyer sur Enter</t>
   </si>
   <si>
-    <t>4.1 Appuyez sur 5 et ensuite Enter</t>
-  </si>
-  <si>
     <t>4.2 Vérifier que votre nom et votre score soient afficher et appuyez sur enter</t>
   </si>
   <si>
@@ -113,12 +106,18 @@
   </si>
   <si>
     <t>6.3 le programme se ferme</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>4.1 Appuyez sur 3 et ensuite Enter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,13 +178,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B4:E26" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B4:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B4:E26" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:E26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Scénario"/>
-    <tableColumn id="2" name="Kenan"/>
-    <tableColumn id="3" name="Arthur_x000a_HP ENVY"/>
-    <tableColumn id="4" name="Léa"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Scénario"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Kenan"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Arthur"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Léa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -487,19 +486,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,120 +506,120 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>